<commit_message>
updated documents and added support form
</commit_message>
<xml_diff>
--- a/documents/MoSCoW.xlsx
+++ b/documents/MoSCoW.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Desktop\USBWebserver v8.6\root\Proftaak-biocodegaming-web\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Desktop\USBWEB\root\Proftaak-biocodegaming-web\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Must</t>
   </si>
@@ -114,13 +114,16 @@
   </si>
   <si>
     <t>inventory(alleen voor owner)</t>
+  </si>
+  <si>
+    <t>?registration?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -149,8 +152,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -173,8 +183,25 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,23 +224,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="2" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="4" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="40% - Accent6" xfId="3" builtinId="51"/>
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -238,7 +284,7 @@
     <tableColumn id="3" name="Could"/>
     <tableColumn id="5" name="Wont"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
 </table>
 </file>
 
@@ -542,18 +588,18 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="29.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.109375" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -562,11 +608,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -577,8 +623,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -588,8 +634,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
@@ -599,7 +645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -610,7 +656,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -621,8 +667,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
@@ -632,15 +678,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>20</v>
       </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -648,7 +697,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -656,12 +705,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
deleted test files, and changed documents
</commit_message>
<xml_diff>
--- a/documents/MoSCoW.xlsx
+++ b/documents/MoSCoW.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Desktop\USBWEB\root\Proftaak-biocodegaming-web\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damia\Dropbox\@USBWebserver v8.6\root\A_PROFTAAK-WEB\Proftaak-biocodegaming-web\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9096"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -83,9 +83,6 @@
     <t>clean design</t>
   </si>
   <si>
-    <t>pm tussen players</t>
-  </si>
-  <si>
     <t>encryption</t>
   </si>
   <si>
@@ -132,6 +129,9 @@
   </si>
   <si>
     <t>inventory moet nog opgemaakt worden</t>
+  </si>
+  <si>
+    <t>Inventory adding</t>
   </si>
 </sst>
 </file>
@@ -586,17 +586,17 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="10.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="10.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -607,10 +607,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>3</v>
       </c>
@@ -621,65 +621,65 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="6"/>
       <c r="G3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>7</v>
       </c>
@@ -690,38 +690,38 @@
         <v>12</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>30</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>9</v>
       </c>
@@ -729,14 +729,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>